<commit_message>
ARD + Non-Functional Requirements - after fixes
</commit_message>
<xml_diff>
--- a/Non-‏‏Functional Requirements.xlsx
+++ b/Non-‏‏Functional Requirements.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Requirment</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
@@ -42,27 +39,9 @@
     <t>The applications will be available 24/7</t>
   </si>
   <si>
-    <t>Multiple users can use the applications at the same time</t>
-  </si>
-  <si>
     <t>Users could use the applications using a browser</t>
   </si>
   <si>
-    <t>The applications will be user friendly</t>
-  </si>
-  <si>
-    <t>Response time will be reasonable</t>
-  </si>
-  <si>
-    <t>The project code could be easly picked up by another software team</t>
-  </si>
-  <si>
-    <t>The system will scale to large amount of data</t>
-  </si>
-  <si>
-    <t>The system will be secured</t>
-  </si>
-  <si>
     <t>The systems components will be independent</t>
   </si>
   <si>
@@ -82,6 +61,15 @@
   </si>
   <si>
     <t>Data will never be permanently deleted from the Database</t>
+  </si>
+  <si>
+    <t>500 users can use the applications at the same time</t>
+  </si>
+  <si>
+    <t>The system will scale to 100 GB of data</t>
+  </si>
+  <si>
+    <t>Requirement</t>
   </si>
 </sst>
 </file>
@@ -436,7 +424,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -453,22 +441,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -476,7 +464,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3">
         <v>5</v>
@@ -489,7 +477,7 @@
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -497,7 +485,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3">
         <v>4</v>
@@ -510,7 +498,7 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -518,7 +506,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3">
         <v>4</v>
@@ -531,7 +519,7 @@
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -539,10 +527,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="3">
         <v>3</v>
@@ -552,7 +540,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -560,10 +548,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -573,7 +561,7 @@
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -581,10 +569,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D7" s="3">
         <v>3</v>
@@ -594,7 +582,7 @@
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -602,20 +590,20 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3">
         <v>5</v>
       </c>
       <c r="D8" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E8" s="4">
         <v>42690</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -623,20 +611,20 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C9" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D9" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E9" s="4">
         <v>42690</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -644,10 +632,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C10" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D10" s="3">
         <v>3</v>
@@ -657,7 +645,7 @@
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -665,110 +653,24 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C11" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E11" s="4">
         <v>42690</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="3">
-        <v>5</v>
-      </c>
-      <c r="D12" s="3">
-        <v>5</v>
-      </c>
-      <c r="E12" s="4">
-        <v>42690</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="3">
-        <v>5</v>
-      </c>
-      <c r="D13" s="3">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4">
-        <v>42690</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="3">
-        <v>5</v>
-      </c>
-      <c r="D14" s="3">
-        <v>3</v>
-      </c>
-      <c r="E14" s="4">
-        <v>42690</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="3">
-        <v>4</v>
-      </c>
-      <c r="D15" s="3">
-        <v>1</v>
-      </c>
-      <c r="E15" s="4">
-        <v>42690</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
+      <c r="A16" s="1"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -776,9 +678,7 @@
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
+      <c r="A17" s="1"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>

</xml_diff>